<commit_message>
Se agrega imagen de Tee Roscado
</commit_message>
<xml_diff>
--- a/publishProductsML/productos.xlsx
+++ b/publishProductsML/productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\OneDrive\Escritorio\Cminox\publishProductsML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60707BC1-A7E7-4BE2-8B82-84CCC54B304A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24048485-3E17-467C-87D2-D0F4C18A3F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
   <si>
     <t>Título</t>
   </si>
@@ -63,49 +63,43 @@
     <t>Envío</t>
   </si>
   <si>
-    <t>MLM191782</t>
-  </si>
-  <si>
     <t>NPT</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/Rick130425/CminoxImages/main/Codo%2045/codo-45-roscado.jpg,http://http2.mlstatic.com/D_743692-MLM47153394760_082021-O.jpg</t>
-  </si>
-  <si>
-    <t>Codo 45° 3/4 150# Acero Inoxidable T-304 Cminox Mty</t>
-  </si>
-  <si>
-    <t>Codo 45° 1 150# Acero Inoxidable T-304 Cminox Mty</t>
-  </si>
-  <si>
-    <t>Codo 45° 1 1/4 150# Acero Inoxidable T-304 Cminox Mty</t>
-  </si>
-  <si>
-    <t>Codo 45° 1 1/2 150# Acero Inoxidable T-304 Cminox Mty</t>
-  </si>
-  <si>
-    <t>Codo 45° 2 150# Acero Inoxidable T-304 Cminox Mty</t>
-  </si>
-  <si>
-    <t>RCND4</t>
-  </si>
-  <si>
-    <t>RCNE4</t>
-  </si>
-  <si>
-    <t>RCN14</t>
-  </si>
-  <si>
-    <t>RCN1B4</t>
-  </si>
-  <si>
-    <t>RCN1D4</t>
-  </si>
-  <si>
-    <t>RCN24</t>
-  </si>
-  <si>
-    <t>Codo Niple 90° 3/4 150# Acero Inoxidable 304</t>
+    <t>https://raw.githubusercontent.com/Rick130425/CminoxImages/main/Codo%20Niple%2090/Codo%20Niple%2090.jpg,http://http2.mlstatic.com/D_743692-MLM47153394760_082021-O.jpg</t>
+  </si>
+  <si>
+    <t>MLM454954</t>
+  </si>
+  <si>
+    <t>RTEB4</t>
+  </si>
+  <si>
+    <t>RTEC4</t>
+  </si>
+  <si>
+    <t>RTED4</t>
+  </si>
+  <si>
+    <t>RTEE4</t>
+  </si>
+  <si>
+    <t>RTE14</t>
+  </si>
+  <si>
+    <t>RTE1B4</t>
+  </si>
+  <si>
+    <t>RTE1D4</t>
+  </si>
+  <si>
+    <t>RTE24</t>
+  </si>
+  <si>
+    <t>RTE34</t>
+  </si>
+  <si>
+    <t>Tee Roscado 1/4 150#, Acero Inoxidable 304</t>
   </si>
 </sst>
 </file>
@@ -501,19 +495,19 @@
   <dimension ref="A1:R61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="60.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.44140625" customWidth="1"/>
-    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.5546875" customWidth="1"/>
-    <col min="5" max="5" width="7.21875" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="54.5546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.6640625" customWidth="1"/>
-    <col min="8" max="8" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.77734375" bestFit="1" customWidth="1"/>
     <col min="11" max="17" width="8.88671875" hidden="1" customWidth="1"/>
@@ -557,146 +551,150 @@
     </row>
     <row r="2" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2">
-        <v>64</v>
+        <f>LEN(A2)</f>
+        <v>42</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D2" s="3">
-        <v>417.59999999999997</v>
+        <v>220.39999999999998</v>
       </c>
       <c r="E2">
-        <v>27</v>
+        <v>220</v>
       </c>
       <c r="F2" t="str">
-        <f t="shared" ref="F2:F7" si="0">A2</f>
-        <v>Codo Niple 90° 3/4 150# Acero Inoxidable 304</v>
+        <f t="shared" ref="F2:F10" si="0">A2</f>
+        <v>Tee Roscado 1/4 150#, Acero Inoxidable 304</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H2" t="s">
         <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="J2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R2" t="str">
         <f>IF(D2&gt;299.99, "Gratis", "Comprador")</f>
-        <v>Gratis</v>
+        <v>Comprador</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B3">
-        <v>74</v>
+        <f t="shared" ref="B3:B10" si="1">LEN(A3)</f>
+        <v>42</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" s="3">
-        <v>556.79999999999995</v>
+        <v>231.99999999999997</v>
       </c>
       <c r="E3">
-        <v>35</v>
+        <v>97</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" si="0"/>
-        <v>Codo 45° 3/4 150# Acero Inoxidable T-304 Cminox Mty</v>
+        <v>Tee Roscado 1/4 150#, Acero Inoxidable 304</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H3" t="s">
         <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="J3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R3" t="str">
-        <f t="shared" ref="R3:R4" si="1">IF(D3&gt;299.99, "Gratis", "Comprador")</f>
-        <v>Gratis</v>
+        <f t="shared" ref="R3:R4" si="2">IF(D3&gt;299.99, "Gratis", "Comprador")</f>
+        <v>Comprador</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B4">
-        <v>20</v>
+        <f t="shared" si="1"/>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D4" s="3">
-        <v>765.59999999999991</v>
+        <v>348</v>
       </c>
       <c r="E4">
-        <v>19</v>
+        <v>135</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" si="0"/>
-        <v>Codo 45° 1 150# Acero Inoxidable T-304 Cminox Mty</v>
+        <v>Tee Roscado 1/4 150#, Acero Inoxidable 304</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H4" t="s">
         <v>6</v>
       </c>
       <c r="I4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R4" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>Gratis</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B5">
-        <v>31</v>
+        <f t="shared" si="1"/>
+        <v>42</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D5" s="3">
-        <v>1276</v>
+        <v>556.79999999999995</v>
       </c>
       <c r="E5">
-        <v>17</v>
+        <v>85</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" si="0"/>
-        <v>Codo 45° 1 1/4 150# Acero Inoxidable T-304 Cminox Mty</v>
+        <v>Tee Roscado 1/4 150#, Acero Inoxidable 304</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H5" t="s">
         <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="J5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R5" t="str">
         <f>IF(D5&gt;299.99, "Gratis", "Comprador")</f>
@@ -705,35 +703,36 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="B6">
-        <v>13</v>
+        <f t="shared" si="1"/>
+        <v>42</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D6" s="3">
-        <v>1484.8</v>
+        <v>765.59999999999991</v>
       </c>
       <c r="E6">
-        <v>7</v>
+        <v>95</v>
       </c>
       <c r="F6" t="str">
         <f t="shared" si="0"/>
-        <v>Codo 45° 1 1/2 150# Acero Inoxidable T-304 Cminox Mty</v>
+        <v>Tee Roscado 1/4 150#, Acero Inoxidable 304</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s">
         <v>6</v>
       </c>
       <c r="I6" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R6" t="str">
         <f>IF(D6&gt;299.99, "Gratis", "Comprador")</f>
@@ -742,35 +741,36 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="B7">
-        <v>11</v>
+        <f t="shared" si="1"/>
+        <v>42</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D7">
-        <v>2134.3999999999996</v>
+        <v>1044</v>
       </c>
       <c r="E7">
         <v>14</v>
       </c>
       <c r="F7" t="str">
         <f t="shared" si="0"/>
-        <v>Codo 45° 2 150# Acero Inoxidable T-304 Cminox Mty</v>
+        <v>Tee Roscado 1/4 150#, Acero Inoxidable 304</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" t="s">
         <v>6</v>
       </c>
       <c r="I7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="J7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="R7" t="str">
         <f>IF(D7&gt;299.99, "Gratis", "Comprador")</f>
@@ -778,13 +778,112 @@
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>1624</v>
+      </c>
+      <c r="E8">
+        <v>52</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="0"/>
+        <v>Tee Roscado 1/4 150#, Acero Inoxidable 304</v>
+      </c>
       <c r="G8" s="1"/>
+      <c r="H8" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" t="s">
+        <v>12</v>
+      </c>
+      <c r="R8" t="str">
+        <f>IF(D8&gt;299.99, "Gratis", "Comprador")</f>
+        <v>Gratis</v>
+      </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>1739.9999999999998</v>
+      </c>
+      <c r="E9">
+        <v>33</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>Tee Roscado 1/4 150#, Acero Inoxidable 304</v>
+      </c>
       <c r="G9" s="1"/>
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" t="s">
+        <v>12</v>
+      </c>
+      <c r="R9" t="str">
+        <f>IF(D9&gt;299.99, "Gratis", "Comprador")</f>
+        <v>Gratis</v>
+      </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>5220</v>
+      </c>
+      <c r="E10">
+        <v>5</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>Tee Roscado 1/4 150#, Acero Inoxidable 304</v>
+      </c>
       <c r="G10" s="1"/>
+      <c r="H10" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" t="s">
+        <v>12</v>
+      </c>
+      <c r="R10" t="str">
+        <f>IF(D10&gt;299.99, "Gratis", "Comprador")</f>
+        <v>Gratis</v>
+      </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G11" s="1"/>
@@ -956,11 +1055,11 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{425C217D-AF77-4E46-81D8-D07D9809338A}"/>
-    <hyperlink ref="G6" r:id="rId2" xr:uid="{FFE9E129-190C-4CA7-8CF5-135567FB7C54}"/>
-    <hyperlink ref="G5" r:id="rId3" xr:uid="{FC4F9A27-EF45-43F2-8FB3-1370AC812262}"/>
-    <hyperlink ref="G4" r:id="rId4" xr:uid="{F920C3C5-84C2-48B3-89E5-0F53D1D1D845}"/>
-    <hyperlink ref="G3" r:id="rId5" xr:uid="{2BD0627C-CE5B-45FA-A38C-3E8F660932FB}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{C2A0776D-8F1E-452B-86CE-5021FC74C957}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{8DF572AE-EB19-4621-8D9E-B993DC9CFBD5}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{21C4C37E-2DCD-40A7-93EC-6432A144CF76}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{0A1F7A97-BE34-48AE-8FE2-9F06EB0E2A3A}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{A04FFC39-607E-4E1C-99AC-71B388CD6934}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{A2BEB788-46D7-41AD-B2FB-D96105464D5B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId7"/>

</xml_diff>

<commit_message>
Se agrega imagenes de Unión H/H y Tapón Cachucha
</commit_message>
<xml_diff>
--- a/publishProductsML/productos.xlsx
+++ b/publishProductsML/productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\OneDrive\Escritorio\Cminox\publishProductsML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24048485-3E17-467C-87D2-D0F4C18A3F5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6373F8AF-3BB4-42A2-94DD-5A103AF7A092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="59">
   <si>
     <t>Título</t>
   </si>
@@ -66,40 +66,142 @@
     <t>NPT</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/Rick130425/CminoxImages/main/Codo%20Niple%2090/Codo%20Niple%2090.jpg,http://http2.mlstatic.com/D_743692-MLM47153394760_082021-O.jpg</t>
-  </si>
-  <si>
     <t>MLM454954</t>
   </si>
   <si>
-    <t>RTEB4</t>
-  </si>
-  <si>
-    <t>RTEC4</t>
-  </si>
-  <si>
-    <t>RTED4</t>
-  </si>
-  <si>
-    <t>RTEE4</t>
-  </si>
-  <si>
-    <t>RTE14</t>
-  </si>
-  <si>
-    <t>RTE1B4</t>
-  </si>
-  <si>
-    <t>RTE1D4</t>
-  </si>
-  <si>
-    <t>RTE24</t>
-  </si>
-  <si>
-    <t>RTE34</t>
-  </si>
-  <si>
-    <t>Tee Roscado 1/4 150#, Acero Inoxidable 304</t>
+    <t>https://raw.githubusercontent.com/Rick130425/CminoxImages/main/Tee%20Roscado/Tee%20Roscado.jpg,http://http2.mlstatic.com/D_743692-MLM47153394760_082021-O.jpg</t>
+  </si>
+  <si>
+    <t>RTUB4</t>
+  </si>
+  <si>
+    <t>RTUC4</t>
+  </si>
+  <si>
+    <t>RTUD4</t>
+  </si>
+  <si>
+    <t>RTUE4</t>
+  </si>
+  <si>
+    <t>RTU14</t>
+  </si>
+  <si>
+    <t>RTU1B4</t>
+  </si>
+  <si>
+    <t>RTU1D4</t>
+  </si>
+  <si>
+    <t>RTU24</t>
+  </si>
+  <si>
+    <t>RTU2D4</t>
+  </si>
+  <si>
+    <t>RTU34</t>
+  </si>
+  <si>
+    <t>RTU44</t>
+  </si>
+  <si>
+    <t>RCBB4</t>
+  </si>
+  <si>
+    <t>RCBC4</t>
+  </si>
+  <si>
+    <t>RCBD4</t>
+  </si>
+  <si>
+    <t>RCBE4</t>
+  </si>
+  <si>
+    <t>RCB14</t>
+  </si>
+  <si>
+    <t>RCB1B4</t>
+  </si>
+  <si>
+    <t>RCB1D4</t>
+  </si>
+  <si>
+    <t>RCB24</t>
+  </si>
+  <si>
+    <t>RCB2D4</t>
+  </si>
+  <si>
+    <t>RCB34</t>
+  </si>
+  <si>
+    <t>RCB44</t>
+  </si>
+  <si>
+    <t>Unión H/H 1/4 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Unión H/H 3/8 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Unión H/H 1/2 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Unión H/H 3/4 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Unión H/H 1 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Unión H/H 1 1/4 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Unión H/H 1 1/2 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Unión H/H 2 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Unión H/H 2 1/2 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Unión H/H 3 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Unión H/H 4 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Tapón Cachucha 1/4 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Tapón Cachucha 3/8 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Tapón Cachucha 1/2 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Tapón Cachucha 3/4 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Tapón Cachucha 1 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Tapón Cachucha 1 1/4 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Tapón Cachucha 1 1/2 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Tapón Cachucha 2 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Tapón Cachucha 2 1/2 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Tapón Cachucha 3 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>Tapón Cachucha 4 150# Acero Inoxidable 304</t>
   </si>
 </sst>
 </file>
@@ -495,7 +597,7 @@
   <dimension ref="A1:R61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -551,27 +653,27 @@
     </row>
     <row r="2" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="B2">
         <f>LEN(A2)</f>
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="3">
+        <v>533.6</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2" t="str">
+        <f t="shared" ref="F2:F23" si="0">A2</f>
+        <v>Unión H/H 1/4 150# Acero Inoxidable 304</v>
+      </c>
+      <c r="G2" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="D2" s="3">
-        <v>220.39999999999998</v>
-      </c>
-      <c r="E2">
-        <v>220</v>
-      </c>
-      <c r="F2" t="str">
-        <f t="shared" ref="F2:F10" si="0">A2</f>
-        <v>Tee Roscado 1/4 150#, Acero Inoxidable 304</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="H2" t="s">
         <v>6</v>
@@ -584,32 +686,32 @@
       </c>
       <c r="R2" t="str">
         <f>IF(D2&gt;299.99, "Gratis", "Comprador")</f>
-        <v>Comprador</v>
+        <v>Gratis</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B10" si="1">LEN(A3)</f>
-        <v>42</v>
+        <f t="shared" ref="B3:B23" si="1">LEN(A3)</f>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="3">
+        <v>603.20000000000005</v>
+      </c>
+      <c r="E3">
+        <v>57</v>
+      </c>
+      <c r="F3" t="str">
+        <f t="shared" si="0"/>
+        <v>Unión H/H 3/8 150# Acero Inoxidable 304</v>
+      </c>
+      <c r="G3" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="D3" s="3">
-        <v>231.99999999999997</v>
-      </c>
-      <c r="E3">
-        <v>97</v>
-      </c>
-      <c r="F3" t="str">
-        <f t="shared" si="0"/>
-        <v>Tee Roscado 1/4 150#, Acero Inoxidable 304</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="H3" t="s">
         <v>6</v>
@@ -621,33 +723,33 @@
         <v>12</v>
       </c>
       <c r="R3" t="str">
-        <f t="shared" ref="R3:R4" si="2">IF(D3&gt;299.99, "Gratis", "Comprador")</f>
-        <v>Comprador</v>
+        <f>IF(D3&gt;299.99, "Gratis", "Comprador")</f>
+        <v>Gratis</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="B4">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="3">
+        <v>696</v>
+      </c>
+      <c r="E4">
+        <v>74</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" si="0"/>
+        <v>Unión H/H 1/2 150# Acero Inoxidable 304</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="D4" s="3">
-        <v>348</v>
-      </c>
-      <c r="E4">
-        <v>135</v>
-      </c>
-      <c r="F4" t="str">
-        <f t="shared" si="0"/>
-        <v>Tee Roscado 1/4 150#, Acero Inoxidable 304</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="H4" t="s">
         <v>6</v>
@@ -659,33 +761,33 @@
         <v>12</v>
       </c>
       <c r="R4" t="str">
-        <f t="shared" si="2"/>
+        <f>IF(D4&gt;299.99, "Gratis", "Comprador")</f>
         <v>Gratis</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="B5">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="3">
+        <v>765.6</v>
+      </c>
+      <c r="E5">
+        <v>41</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="0"/>
+        <v>Unión H/H 3/4 150# Acero Inoxidable 304</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="D5" s="3">
-        <v>556.79999999999995</v>
-      </c>
-      <c r="E5">
-        <v>85</v>
-      </c>
-      <c r="F5" t="str">
-        <f t="shared" si="0"/>
-        <v>Tee Roscado 1/4 150#, Acero Inoxidable 304</v>
-      </c>
-      <c r="G5" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="H5" t="s">
         <v>6</v>
@@ -703,27 +805,27 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
       <c r="B6">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="3">
+        <v>1624</v>
+      </c>
+      <c r="E6">
+        <v>71</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>Unión H/H 1 150# Acero Inoxidable 304</v>
+      </c>
+      <c r="G6" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="D6" s="3">
-        <v>765.59999999999991</v>
-      </c>
-      <c r="E6">
-        <v>95</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="0"/>
-        <v>Tee Roscado 1/4 150#, Acero Inoxidable 304</v>
-      </c>
-      <c r="G6" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="H6" t="s">
         <v>6</v>
@@ -741,27 +843,27 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
       <c r="B7">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>1856</v>
+      </c>
+      <c r="E7">
+        <v>28</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="0"/>
+        <v>Unión H/H 1 1/4 150# Acero Inoxidable 304</v>
+      </c>
+      <c r="G7" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="D7">
-        <v>1044</v>
-      </c>
-      <c r="E7">
-        <v>14</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" si="0"/>
-        <v>Tee Roscado 1/4 150#, Acero Inoxidable 304</v>
-      </c>
-      <c r="G7" s="6" t="s">
-        <v>13</v>
       </c>
       <c r="H7" t="s">
         <v>6</v>
@@ -779,26 +881,28 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="B8">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8">
-        <v>1624</v>
+        <v>2088</v>
       </c>
       <c r="E8">
         <v>52</v>
       </c>
       <c r="F8" t="str">
         <f t="shared" si="0"/>
-        <v>Tee Roscado 1/4 150#, Acero Inoxidable 304</v>
-      </c>
-      <c r="G8" s="1"/>
+        <v>Unión H/H 1 1/2 150# Acero Inoxidable 304</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>14</v>
+      </c>
       <c r="H8" t="s">
         <v>6</v>
       </c>
@@ -815,26 +919,28 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="B9">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9">
+        <v>2296.8000000000002</v>
+      </c>
+      <c r="E9">
+        <v>15</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="0"/>
+        <v>Unión H/H 2 150# Acero Inoxidable 304</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D9">
-        <v>1739.9999999999998</v>
-      </c>
-      <c r="E9">
-        <v>33</v>
-      </c>
-      <c r="F9" t="str">
-        <f t="shared" si="0"/>
-        <v>Tee Roscado 1/4 150#, Acero Inoxidable 304</v>
-      </c>
-      <c r="G9" s="1"/>
       <c r="H9" t="s">
         <v>6</v>
       </c>
@@ -851,26 +957,28 @@
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>24</v>
+        <v>45</v>
       </c>
       <c r="B10">
         <f t="shared" si="1"/>
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10">
+        <v>4408</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="0"/>
+        <v>Unión H/H 2 1/2 150# Acero Inoxidable 304</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D10">
-        <v>5220</v>
-      </c>
-      <c r="E10">
-        <v>5</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>Tee Roscado 1/4 150#, Acero Inoxidable 304</v>
-      </c>
-      <c r="G10" s="1"/>
       <c r="H10" t="s">
         <v>6</v>
       </c>
@@ -886,127 +994,547 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>5800</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="0"/>
+        <v>Unión H/H 3 150# Acero Inoxidable 304</v>
+      </c>
       <c r="G11" s="1"/>
+      <c r="H11" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" t="s">
+        <v>12</v>
+      </c>
+      <c r="R11" t="str">
+        <f t="shared" ref="R11:R22" si="2">IF(D11&gt;299.99, "Gratis", "Comprador")</f>
+        <v>Gratis</v>
+      </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12">
+        <f t="shared" si="1"/>
+        <v>37</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>6960</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="str">
+        <f t="shared" si="0"/>
+        <v>Unión H/H 4 150# Acero Inoxidable 304</v>
+      </c>
       <c r="G12" s="1"/>
+      <c r="H12" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" t="s">
+        <v>12</v>
+      </c>
+      <c r="R12" t="str">
+        <f t="shared" si="2"/>
+        <v>Gratis</v>
+      </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="C13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D13">
+        <v>116</v>
+      </c>
+      <c r="E13">
+        <v>50</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" si="0"/>
+        <v>Tapón Cachucha 1/4 150# Acero Inoxidable 304</v>
+      </c>
       <c r="G13" s="1"/>
+      <c r="H13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" t="s">
+        <v>12</v>
+      </c>
+      <c r="R13" t="str">
+        <f t="shared" si="2"/>
+        <v>Comprador</v>
+      </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="C14" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <v>157.76</v>
+      </c>
+      <c r="E14">
+        <v>33</v>
+      </c>
+      <c r="F14" t="str">
+        <f t="shared" si="0"/>
+        <v>Tapón Cachucha 3/8 150# Acero Inoxidable 304</v>
+      </c>
       <c r="G14" s="1"/>
+      <c r="H14" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" t="s">
+        <v>12</v>
+      </c>
+      <c r="R14" t="str">
+        <f t="shared" si="2"/>
+        <v>Comprador</v>
+      </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>50</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>167.04</v>
+      </c>
+      <c r="E15">
+        <v>146</v>
+      </c>
+      <c r="F15" t="str">
+        <f t="shared" si="0"/>
+        <v>Tapón Cachucha 1/2 150# Acero Inoxidable 304</v>
+      </c>
       <c r="G15" s="1"/>
+      <c r="H15" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" t="s">
+        <v>12</v>
+      </c>
+      <c r="R15" t="str">
+        <f t="shared" si="2"/>
+        <v>Comprador</v>
+      </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>51</v>
+      </c>
+      <c r="B16">
+        <f t="shared" si="1"/>
+        <v>44</v>
+      </c>
+      <c r="C16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D16">
+        <v>180.96</v>
+      </c>
+      <c r="E16">
+        <v>45</v>
+      </c>
+      <c r="F16" t="str">
+        <f t="shared" si="0"/>
+        <v>Tapón Cachucha 3/4 150# Acero Inoxidable 304</v>
+      </c>
       <c r="G16" s="1"/>
-    </row>
-    <row r="17" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>6</v>
+      </c>
+      <c r="I16" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" t="s">
+        <v>12</v>
+      </c>
+      <c r="R16" t="str">
+        <f t="shared" si="2"/>
+        <v>Comprador</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B17">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="C17" t="s">
+        <v>13</v>
+      </c>
+      <c r="D17">
+        <v>301.60000000000002</v>
+      </c>
+      <c r="E17">
+        <v>98</v>
+      </c>
+      <c r="F17" t="str">
+        <f t="shared" si="0"/>
+        <v>Tapón Cachucha 1 150# Acero Inoxidable 304</v>
+      </c>
       <c r="G17" s="1"/>
-    </row>
-    <row r="18" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" t="s">
+        <v>12</v>
+      </c>
+      <c r="R17" t="str">
+        <f t="shared" si="2"/>
+        <v>Gratis</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B18">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>13</v>
+      </c>
+      <c r="D18">
+        <v>464</v>
+      </c>
+      <c r="E18">
+        <v>17</v>
+      </c>
+      <c r="F18" t="str">
+        <f t="shared" si="0"/>
+        <v>Tapón Cachucha 1 1/4 150# Acero Inoxidable 304</v>
+      </c>
       <c r="G18" s="1"/>
-    </row>
-    <row r="19" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>6</v>
+      </c>
+      <c r="I18" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" t="s">
+        <v>12</v>
+      </c>
+      <c r="R18" t="str">
+        <f t="shared" si="2"/>
+        <v>Gratis</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19">
+        <v>719.2</v>
+      </c>
+      <c r="E19">
+        <v>34</v>
+      </c>
+      <c r="F19" t="str">
+        <f t="shared" si="0"/>
+        <v>Tapón Cachucha 1 1/2 150# Acero Inoxidable 304</v>
+      </c>
       <c r="G19" s="1"/>
-    </row>
-    <row r="20" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19" t="s">
+        <v>12</v>
+      </c>
+      <c r="R19" t="str">
+        <f t="shared" si="2"/>
+        <v>Gratis</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20">
+        <v>858.4</v>
+      </c>
+      <c r="E20">
+        <v>22</v>
+      </c>
+      <c r="F20" t="str">
+        <f t="shared" si="0"/>
+        <v>Tapón Cachucha 2 150# Acero Inoxidable 304</v>
+      </c>
       <c r="G20" s="1"/>
-    </row>
-    <row r="21" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>6</v>
+      </c>
+      <c r="I20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J20" t="s">
+        <v>12</v>
+      </c>
+      <c r="R20" t="str">
+        <f t="shared" si="2"/>
+        <v>Gratis</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>56</v>
+      </c>
+      <c r="B21">
+        <f t="shared" si="1"/>
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>13</v>
+      </c>
+      <c r="D21">
+        <v>1392</v>
+      </c>
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21" t="str">
+        <f t="shared" si="0"/>
+        <v>Tapón Cachucha 2 1/2 150# Acero Inoxidable 304</v>
+      </c>
       <c r="G21" s="1"/>
-    </row>
-    <row r="22" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>6</v>
+      </c>
+      <c r="I21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J21" t="s">
+        <v>12</v>
+      </c>
+      <c r="R21" t="str">
+        <f t="shared" si="2"/>
+        <v>Gratis</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22">
+        <v>2273.6</v>
+      </c>
+      <c r="E22">
+        <v>6</v>
+      </c>
+      <c r="F22" t="str">
+        <f t="shared" si="0"/>
+        <v>Tapón Cachucha 3 150# Acero Inoxidable 304</v>
+      </c>
       <c r="G22" s="1"/>
-    </row>
-    <row r="23" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D23" s="3"/>
+      <c r="H22" t="s">
+        <v>6</v>
+      </c>
+      <c r="I22" t="s">
+        <v>35</v>
+      </c>
+      <c r="J22" t="s">
+        <v>12</v>
+      </c>
+      <c r="R22" t="str">
+        <f t="shared" si="2"/>
+        <v>Gratis</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>58</v>
+      </c>
+      <c r="B23">
+        <f t="shared" si="1"/>
+        <v>42</v>
+      </c>
+      <c r="C23" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23">
+        <v>3016</v>
+      </c>
+      <c r="E23">
+        <v>8</v>
+      </c>
+      <c r="F23" t="str">
+        <f t="shared" si="0"/>
+        <v>Tapón Cachucha 4 150# Acero Inoxidable 304</v>
+      </c>
       <c r="G23" s="1"/>
-    </row>
-    <row r="24" spans="4:7" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>6</v>
+      </c>
+      <c r="I23" t="s">
+        <v>36</v>
+      </c>
+      <c r="J23" t="s">
+        <v>12</v>
+      </c>
+      <c r="R23" t="str">
+        <f>IF(D23&gt;299.99, "Gratis", "Comprador")</f>
+        <v>Gratis</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G25" s="1"/>
     </row>
-    <row r="26" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="D26" s="3"/>
       <c r="G26" s="1"/>
     </row>
-    <row r="27" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G27" s="1"/>
     </row>
-    <row r="28" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G28" s="1"/>
     </row>
-    <row r="29" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D29" s="3"/>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G29" s="1"/>
     </row>
-    <row r="30" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G30" s="1"/>
     </row>
-    <row r="31" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G31" s="1"/>
     </row>
-    <row r="32" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D32" s="3"/>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="G32" s="1"/>
     </row>
-    <row r="33" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G33" s="1"/>
     </row>
-    <row r="34" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G34" s="1"/>
     </row>
-    <row r="35" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D35" s="3"/>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G35" s="4"/>
     </row>
-    <row r="36" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G36" s="1"/>
     </row>
-    <row r="37" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D37" s="3"/>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G37" s="4"/>
     </row>
-    <row r="38" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G38" s="1"/>
     </row>
-    <row r="39" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D39" s="3"/>
+    <row r="39" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G39" s="4"/>
     </row>
-    <row r="40" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G40" s="1"/>
     </row>
-    <row r="41" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D41" s="3"/>
+    <row r="41" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G41" s="4"/>
     </row>
-    <row r="42" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G42" s="1"/>
     </row>
-    <row r="43" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D43" s="3"/>
+    <row r="43" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G43" s="4"/>
     </row>
-    <row r="44" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G44" s="1"/>
     </row>
-    <row r="45" spans="4:7" x14ac:dyDescent="0.3">
-      <c r="D45" s="3"/>
+    <row r="45" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G45" s="4"/>
     </row>
-    <row r="46" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G46" s="1"/>
     </row>
-    <row r="47" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G47" s="4"/>
     </row>
-    <row r="48" spans="4:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="7:7" x14ac:dyDescent="0.3">
       <c r="G48" s="1"/>
     </row>
     <row r="49" spans="4:7" x14ac:dyDescent="0.3">
@@ -1055,13 +1583,16 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{425C217D-AF77-4E46-81D8-D07D9809338A}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{8DF572AE-EB19-4621-8D9E-B993DC9CFBD5}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{21C4C37E-2DCD-40A7-93EC-6432A144CF76}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{0A1F7A97-BE34-48AE-8FE2-9F06EB0E2A3A}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{A04FFC39-607E-4E1C-99AC-71B388CD6934}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{A2BEB788-46D7-41AD-B2FB-D96105464D5B}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{B67FCD9A-9E78-4CC6-A52B-D065B7E5D7AC}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{7413D119-62F2-4781-A4C6-DEFF016D8F98}"/>
+    <hyperlink ref="G5" r:id="rId4" xr:uid="{9838D750-5EF0-47A8-BB0E-8319676D6D6E}"/>
+    <hyperlink ref="G6" r:id="rId5" xr:uid="{2CBE13FE-3075-4B5A-86DD-29C3D78F7FAC}"/>
+    <hyperlink ref="G7" r:id="rId6" xr:uid="{DD87ECE6-D619-4875-8078-478ED4FFCC6C}"/>
+    <hyperlink ref="G8" r:id="rId7" xr:uid="{ED388FBB-6A71-497C-9B1D-92A204C30D6F}"/>
+    <hyperlink ref="G9" r:id="rId8" xr:uid="{B45E0BFC-07AC-4F23-8339-C403FA4F154F}"/>
+    <hyperlink ref="G10" r:id="rId9" xr:uid="{74B5303E-B50B-46B7-8B08-39AE9E069A59}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega imagen de Reducción Campana
</commit_message>
<xml_diff>
--- a/publishProductsML/productos.xlsx
+++ b/publishProductsML/productos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricar\OneDrive\Escritorio\Cminox\publishProductsML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6373F8AF-3BB4-42A2-94DD-5A103AF7A092}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2D1F64-D234-4099-812D-C1889B358B93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="60">
   <si>
     <t>Título</t>
   </si>
@@ -69,9 +69,6 @@
     <t>MLM454954</t>
   </si>
   <si>
-    <t>https://raw.githubusercontent.com/Rick130425/CminoxImages/main/Tee%20Roscado/Tee%20Roscado.jpg,http://http2.mlstatic.com/D_743692-MLM47153394760_082021-O.jpg</t>
-  </si>
-  <si>
     <t>RTUB4</t>
   </si>
   <si>
@@ -202,6 +199,12 @@
   </si>
   <si>
     <t>Tapón Cachucha 4 150# Acero Inoxidable 304</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Rick130425/CminoxImages/main/Uni%C3%B3n%20H-H/union-hh.jpg,http://http2.mlstatic.com/D_743692-MLM47153394760_082021-O.jpg</t>
+  </si>
+  <si>
+    <t>https://raw.githubusercontent.com/Rick130425/CminoxImages/main/Tap%C3%B3n%20Cachuca/Tap%C3%B3n%20Cachucha.jpg,http://http2.mlstatic.com/D_743692-MLM47153394760_082021-O.jpg</t>
   </si>
 </sst>
 </file>
@@ -597,7 +600,7 @@
   <dimension ref="A1:R61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -653,7 +656,7 @@
     </row>
     <row r="2" spans="1:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B2">
         <f>LEN(A2)</f>
@@ -673,28 +676,28 @@
         <v>Unión H/H 1/4 150# Acero Inoxidable 304</v>
       </c>
       <c r="G2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I2" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
-        <v>6</v>
-      </c>
-      <c r="I2" t="s">
-        <v>15</v>
-      </c>
       <c r="J2" t="s">
         <v>12</v>
       </c>
       <c r="R2" t="str">
-        <f>IF(D2&gt;299.99, "Gratis", "Comprador")</f>
+        <f t="shared" ref="R2:R10" si="1">IF(D2&gt;299.99, "Gratis", "Comprador")</f>
         <v>Gratis</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B3">
-        <f t="shared" ref="B3:B23" si="1">LEN(A3)</f>
+        <f t="shared" ref="B3:B23" si="2">LEN(A3)</f>
         <v>39</v>
       </c>
       <c r="C3" t="s">
@@ -711,28 +714,28 @@
         <v>Unión H/H 3/8 150# Acero Inoxidable 304</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="H3" t="s">
         <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="J3" t="s">
         <v>12</v>
       </c>
       <c r="R3" t="str">
-        <f>IF(D3&gt;299.99, "Gratis", "Comprador")</f>
+        <f t="shared" si="1"/>
         <v>Gratis</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="C4" t="s">
@@ -749,28 +752,28 @@
         <v>Unión H/H 1/2 150# Acero Inoxidable 304</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="H4" t="s">
         <v>6</v>
       </c>
       <c r="I4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J4" t="s">
         <v>12</v>
       </c>
       <c r="R4" t="str">
-        <f>IF(D4&gt;299.99, "Gratis", "Comprador")</f>
+        <f t="shared" si="1"/>
         <v>Gratis</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>39</v>
       </c>
       <c r="C5" t="s">
@@ -787,28 +790,28 @@
         <v>Unión H/H 3/4 150# Acero Inoxidable 304</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="H5" t="s">
         <v>6</v>
       </c>
       <c r="I5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="J5" t="s">
         <v>12</v>
       </c>
       <c r="R5" t="str">
-        <f>IF(D5&gt;299.99, "Gratis", "Comprador")</f>
+        <f t="shared" si="1"/>
         <v>Gratis</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="C6" t="s">
@@ -825,28 +828,28 @@
         <v>Unión H/H 1 150# Acero Inoxidable 304</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="H6" t="s">
         <v>6</v>
       </c>
       <c r="I6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="J6" t="s">
         <v>12</v>
       </c>
       <c r="R6" t="str">
-        <f>IF(D6&gt;299.99, "Gratis", "Comprador")</f>
+        <f t="shared" si="1"/>
         <v>Gratis</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="C7" t="s">
@@ -863,28 +866,28 @@
         <v>Unión H/H 1 1/4 150# Acero Inoxidable 304</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="H7" t="s">
         <v>6</v>
       </c>
       <c r="I7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="J7" t="s">
         <v>12</v>
       </c>
       <c r="R7" t="str">
-        <f>IF(D7&gt;299.99, "Gratis", "Comprador")</f>
+        <f t="shared" si="1"/>
         <v>Gratis</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="C8" t="s">
@@ -901,28 +904,28 @@
         <v>Unión H/H 1 1/2 150# Acero Inoxidable 304</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="H8" t="s">
         <v>6</v>
       </c>
       <c r="I8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="J8" t="s">
         <v>12</v>
       </c>
       <c r="R8" t="str">
-        <f>IF(D8&gt;299.99, "Gratis", "Comprador")</f>
+        <f t="shared" si="1"/>
         <v>Gratis</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="C9" t="s">
@@ -939,28 +942,28 @@
         <v>Unión H/H 2 150# Acero Inoxidable 304</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="H9" t="s">
         <v>6</v>
       </c>
       <c r="I9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J9" t="s">
         <v>12</v>
       </c>
       <c r="R9" t="str">
-        <f>IF(D9&gt;299.99, "Gratis", "Comprador")</f>
+        <f t="shared" si="1"/>
         <v>Gratis</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>41</v>
       </c>
       <c r="C10" t="s">
@@ -977,28 +980,28 @@
         <v>Unión H/H 2 1/2 150# Acero Inoxidable 304</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>14</v>
+        <v>58</v>
       </c>
       <c r="H10" t="s">
         <v>6</v>
       </c>
       <c r="I10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="J10" t="s">
         <v>12</v>
       </c>
       <c r="R10" t="str">
-        <f>IF(D10&gt;299.99, "Gratis", "Comprador")</f>
+        <f t="shared" si="1"/>
         <v>Gratis</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="C11" t="s">
@@ -1014,27 +1017,29 @@
         <f t="shared" si="0"/>
         <v>Unión H/H 3 150# Acero Inoxidable 304</v>
       </c>
-      <c r="G11" s="1"/>
+      <c r="G11" s="6" t="s">
+        <v>58</v>
+      </c>
       <c r="H11" t="s">
         <v>6</v>
       </c>
       <c r="I11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="J11" t="s">
         <v>12</v>
       </c>
       <c r="R11" t="str">
-        <f t="shared" ref="R11:R22" si="2">IF(D11&gt;299.99, "Gratis", "Comprador")</f>
+        <f t="shared" ref="R11:R22" si="3">IF(D11&gt;299.99, "Gratis", "Comprador")</f>
         <v>Gratis</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>37</v>
       </c>
       <c r="C12" t="s">
@@ -1050,27 +1055,29 @@
         <f t="shared" si="0"/>
         <v>Unión H/H 4 150# Acero Inoxidable 304</v>
       </c>
-      <c r="G12" s="1"/>
+      <c r="G12" s="6" t="s">
+        <v>58</v>
+      </c>
       <c r="H12" t="s">
         <v>6</v>
       </c>
       <c r="I12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J12" t="s">
         <v>12</v>
       </c>
       <c r="R12" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Gratis</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="C13" t="s">
@@ -1086,27 +1093,29 @@
         <f t="shared" si="0"/>
         <v>Tapón Cachucha 1/4 150# Acero Inoxidable 304</v>
       </c>
-      <c r="G13" s="1"/>
+      <c r="G13" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="H13" t="s">
         <v>6</v>
       </c>
       <c r="I13" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="J13" t="s">
         <v>12</v>
       </c>
       <c r="R13" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Comprador</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="C14" t="s">
@@ -1122,27 +1131,29 @@
         <f t="shared" si="0"/>
         <v>Tapón Cachucha 3/8 150# Acero Inoxidable 304</v>
       </c>
-      <c r="G14" s="1"/>
+      <c r="G14" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="H14" t="s">
         <v>6</v>
       </c>
       <c r="I14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="J14" t="s">
         <v>12</v>
       </c>
       <c r="R14" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Comprador</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="C15" t="s">
@@ -1158,27 +1169,29 @@
         <f t="shared" si="0"/>
         <v>Tapón Cachucha 1/2 150# Acero Inoxidable 304</v>
       </c>
-      <c r="G15" s="1"/>
+      <c r="G15" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="H15" t="s">
         <v>6</v>
       </c>
       <c r="I15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J15" t="s">
         <v>12</v>
       </c>
       <c r="R15" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Comprador</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="C16" t="s">
@@ -1194,27 +1207,29 @@
         <f t="shared" si="0"/>
         <v>Tapón Cachucha 3/4 150# Acero Inoxidable 304</v>
       </c>
-      <c r="G16" s="1"/>
+      <c r="G16" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="H16" t="s">
         <v>6</v>
       </c>
       <c r="I16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J16" t="s">
         <v>12</v>
       </c>
       <c r="R16" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Comprador</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="C17" t="s">
@@ -1230,27 +1245,29 @@
         <f t="shared" si="0"/>
         <v>Tapón Cachucha 1 150# Acero Inoxidable 304</v>
       </c>
-      <c r="G17" s="1"/>
+      <c r="G17" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="H17" t="s">
         <v>6</v>
       </c>
       <c r="I17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="J17" t="s">
         <v>12</v>
       </c>
       <c r="R17" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Gratis</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
       <c r="C18" t="s">
@@ -1266,27 +1283,29 @@
         <f t="shared" si="0"/>
         <v>Tapón Cachucha 1 1/4 150# Acero Inoxidable 304</v>
       </c>
-      <c r="G18" s="1"/>
+      <c r="G18" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="H18" t="s">
         <v>6</v>
       </c>
       <c r="I18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J18" t="s">
         <v>12</v>
       </c>
       <c r="R18" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Gratis</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
       <c r="C19" t="s">
@@ -1302,27 +1321,29 @@
         <f t="shared" si="0"/>
         <v>Tapón Cachucha 1 1/2 150# Acero Inoxidable 304</v>
       </c>
-      <c r="G19" s="1"/>
+      <c r="G19" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="H19" t="s">
         <v>6</v>
       </c>
       <c r="I19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="J19" t="s">
         <v>12</v>
       </c>
       <c r="R19" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Gratis</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="C20" t="s">
@@ -1338,27 +1359,29 @@
         <f t="shared" si="0"/>
         <v>Tapón Cachucha 2 150# Acero Inoxidable 304</v>
       </c>
-      <c r="G20" s="1"/>
+      <c r="G20" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="H20" t="s">
         <v>6</v>
       </c>
       <c r="I20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J20" t="s">
         <v>12</v>
       </c>
       <c r="R20" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Gratis</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>46</v>
       </c>
       <c r="C21" t="s">
@@ -1374,27 +1397,29 @@
         <f t="shared" si="0"/>
         <v>Tapón Cachucha 2 1/2 150# Acero Inoxidable 304</v>
       </c>
-      <c r="G21" s="1"/>
+      <c r="G21" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="H21" t="s">
         <v>6</v>
       </c>
       <c r="I21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J21" t="s">
         <v>12</v>
       </c>
       <c r="R21" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Gratis</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="C22" t="s">
@@ -1410,27 +1435,29 @@
         <f t="shared" si="0"/>
         <v>Tapón Cachucha 3 150# Acero Inoxidable 304</v>
       </c>
-      <c r="G22" s="1"/>
+      <c r="G22" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="H22" t="s">
         <v>6</v>
       </c>
       <c r="I22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J22" t="s">
         <v>12</v>
       </c>
       <c r="R22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>Gratis</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>42</v>
       </c>
       <c r="C23" t="s">
@@ -1446,12 +1473,14 @@
         <f t="shared" si="0"/>
         <v>Tapón Cachucha 4 150# Acero Inoxidable 304</v>
       </c>
-      <c r="G23" s="1"/>
+      <c r="G23" s="6" t="s">
+        <v>59</v>
+      </c>
       <c r="H23" t="s">
         <v>6</v>
       </c>
       <c r="I23" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J23" t="s">
         <v>12</v>
@@ -1583,16 +1612,30 @@
   <phoneticPr fontId="3" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{425C217D-AF77-4E46-81D8-D07D9809338A}"/>
-    <hyperlink ref="G3" r:id="rId2" xr:uid="{B67FCD9A-9E78-4CC6-A52B-D065B7E5D7AC}"/>
-    <hyperlink ref="G4" r:id="rId3" xr:uid="{7413D119-62F2-4781-A4C6-DEFF016D8F98}"/>
-    <hyperlink ref="G5" r:id="rId4" xr:uid="{9838D750-5EF0-47A8-BB0E-8319676D6D6E}"/>
-    <hyperlink ref="G6" r:id="rId5" xr:uid="{2CBE13FE-3075-4B5A-86DD-29C3D78F7FAC}"/>
-    <hyperlink ref="G7" r:id="rId6" xr:uid="{DD87ECE6-D619-4875-8078-478ED4FFCC6C}"/>
-    <hyperlink ref="G8" r:id="rId7" xr:uid="{ED388FBB-6A71-497C-9B1D-92A204C30D6F}"/>
-    <hyperlink ref="G9" r:id="rId8" xr:uid="{B45E0BFC-07AC-4F23-8339-C403FA4F154F}"/>
-    <hyperlink ref="G10" r:id="rId9" xr:uid="{74B5303E-B50B-46B7-8B08-39AE9E069A59}"/>
+    <hyperlink ref="G3" r:id="rId2" xr:uid="{58BEB2A0-B790-42C8-B306-DD42F4C563C5}"/>
+    <hyperlink ref="G4" r:id="rId3" xr:uid="{7A862649-778F-4CC2-9B12-9F76BEF9A65D}"/>
+    <hyperlink ref="G6" r:id="rId4" xr:uid="{42BC4CA0-2BC3-4043-A12E-27533D04C466}"/>
+    <hyperlink ref="G8" r:id="rId5" xr:uid="{AE00F725-2CC1-45F8-BEE8-0C72474C9261}"/>
+    <hyperlink ref="G10" r:id="rId6" xr:uid="{E25E96FD-613A-4930-9DFE-010A54CD1A83}"/>
+    <hyperlink ref="G5" r:id="rId7" xr:uid="{4C3CCF6D-E907-413B-99F1-93D19D714DA5}"/>
+    <hyperlink ref="G7" r:id="rId8" xr:uid="{262EF6CD-2DBF-4179-95D7-1B36989DE9DB}"/>
+    <hyperlink ref="G9" r:id="rId9" xr:uid="{511AB3B5-ACA5-4E0F-8DEB-1ED0234AC2EB}"/>
+    <hyperlink ref="G12" r:id="rId10" xr:uid="{7742CD02-154C-44A5-B067-1BC42F641C22}"/>
+    <hyperlink ref="A1" r:id="rId11" display="https://raw.githubusercontent.com/Rick130425/CminoxImages/main/Uni%C3%B3n%20H-H/union-hh.jpg,http://http2.mlstatic.com/D_743692-MLM47153394760_082021-O.jpg" xr:uid="{4788E73E-E55B-4149-9710-8CF10E4DBB2E}"/>
+    <hyperlink ref="G11" r:id="rId12" xr:uid="{3CE7E341-40F3-4398-9C20-18D6088AF38E}"/>
+    <hyperlink ref="G13" r:id="rId13" xr:uid="{87218BEB-3774-40F3-B5B7-204C881CEE2F}"/>
+    <hyperlink ref="G14" r:id="rId14" xr:uid="{55199D87-5FB2-4E42-B8C6-5B6DE8273A31}"/>
+    <hyperlink ref="G15" r:id="rId15" xr:uid="{01470898-386B-4138-9EEB-00EAFA36D16F}"/>
+    <hyperlink ref="G17" r:id="rId16" xr:uid="{4DD621A5-6A60-4076-934A-7526C0C9A39B}"/>
+    <hyperlink ref="G19" r:id="rId17" xr:uid="{1D8E3D7C-0BCB-4755-92B5-11242B69EAED}"/>
+    <hyperlink ref="G21" r:id="rId18" xr:uid="{D10A77E7-62DE-4298-BE00-137443B1C65B}"/>
+    <hyperlink ref="G23" r:id="rId19" xr:uid="{A53D6866-DF23-4931-9A77-3CA541EA7DE8}"/>
+    <hyperlink ref="G16" r:id="rId20" xr:uid="{ADF3EF26-67CA-4FB4-B82A-7601E675CE33}"/>
+    <hyperlink ref="G18" r:id="rId21" xr:uid="{B7D4E1B6-DC66-44D9-BEEF-DF852B173CDF}"/>
+    <hyperlink ref="G20" r:id="rId22" xr:uid="{8CFC1E6D-E5AC-4A76-B30F-14C1775A1DA6}"/>
+    <hyperlink ref="G22" r:id="rId23" xr:uid="{A0132EBE-936E-4D83-92D9-38745025B308}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
</xml_diff>